<commit_message>
Edits to depth mapper and test notebook.
</commit_message>
<xml_diff>
--- a/CB_03_depth_map_qual_results.xlsx
+++ b/CB_03_depth_map_qual_results.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rmccune\depth_mapping_updated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FA63809-6003-4CA0-AB6B-61F13C32430E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AA0E09-D466-412D-95FE-B35F6B2D5DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBD90A7E-A1B8-4AD2-918B-86DF11A7BBD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$1:$D$56</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -352,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,8 +364,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,7 +701,7 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +710,7 @@
     <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -725,7 +726,7 @@
       <c r="D1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -742,7 +743,7 @@
       <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -759,7 +760,7 @@
       <c r="D3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" t="s">
         <v>60</v>
       </c>
     </row>
@@ -776,7 +777,7 @@
       <c r="D4" s="1">
         <v>0</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" t="s">
         <v>59</v>
       </c>
     </row>
@@ -793,7 +794,7 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" t="s">
         <v>59</v>
       </c>
     </row>
@@ -810,7 +811,7 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" t="s">
         <v>59</v>
       </c>
     </row>
@@ -827,7 +828,7 @@
       <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" t="s">
         <v>59</v>
       </c>
     </row>
@@ -844,7 +845,7 @@
       <c r="D8" s="1">
         <v>0</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" t="s">
         <v>62</v>
       </c>
     </row>
@@ -861,7 +862,7 @@
       <c r="D9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" t="s">
         <v>64</v>
       </c>
     </row>
@@ -878,7 +879,7 @@
       <c r="D10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" t="s">
         <v>65</v>
       </c>
     </row>
@@ -895,7 +896,7 @@
       <c r="D11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" t="s">
         <v>65</v>
       </c>
     </row>
@@ -912,7 +913,7 @@
       <c r="D12" s="1">
         <v>0</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" t="s">
         <v>66</v>
       </c>
     </row>
@@ -929,7 +930,7 @@
       <c r="D13" s="1">
         <v>0</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" t="s">
         <v>67</v>
       </c>
     </row>
@@ -946,7 +947,7 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" t="s">
         <v>68</v>
       </c>
     </row>
@@ -963,7 +964,7 @@
       <c r="D15" s="1">
         <v>0</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" t="s">
         <v>69</v>
       </c>
     </row>
@@ -980,7 +981,7 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" t="s">
         <v>70</v>
       </c>
     </row>
@@ -997,7 +998,7 @@
       <c r="D17" s="1">
         <v>0</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1014,7 +1015,7 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1031,7 +1032,7 @@
       <c r="D19" s="1">
         <v>0</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1062,7 +1063,7 @@
       <c r="D21" s="1">
         <v>0</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1079,7 +1080,7 @@
       <c r="D22" s="1">
         <v>1</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1124,7 +1125,7 @@
       <c r="D25" s="1">
         <v>0</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1141,7 +1142,7 @@
       <c r="D26" s="1">
         <v>0</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1158,7 +1159,7 @@
       <c r="D27" s="1">
         <v>1</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1175,7 +1176,7 @@
       <c r="D28" s="1">
         <v>1</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1234,7 +1235,7 @@
       <c r="D32" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1335,7 +1336,7 @@
       <c r="D39" s="1">
         <v>0</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1352,7 +1353,7 @@
       <c r="D40" s="1">
         <v>0</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1369,7 +1370,7 @@
       <c r="D41" s="1">
         <v>0</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1386,7 +1387,7 @@
       <c r="D42" s="1">
         <v>1</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1403,7 +1404,7 @@
       <c r="D43" s="1">
         <v>1</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1420,7 +1421,7 @@
       <c r="D44" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E44" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1437,7 +1438,7 @@
       <c r="D45" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1454,7 +1455,7 @@
       <c r="D46" s="1">
         <v>0</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1471,7 +1472,7 @@
       <c r="D47" s="1">
         <v>1</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1502,7 +1503,7 @@
       <c r="D49" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1519,7 +1520,7 @@
       <c r="D50" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E50" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1550,7 +1551,7 @@
       <c r="D52" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E52" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1581,7 +1582,7 @@
       <c r="D54" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="E54" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1614,6 +1615,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="D1:D56" xr:uid="{2AA25543-DF5E-4343-8E5C-A4DA120CCB4B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>